<commit_message>
Atualizado por script em 26-10-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/poland_division-2_2023-2024.xlsx
+++ b/2023/poland_division-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V123"/>
+  <dimension ref="A1:V124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,22 +941,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Wisla Pulawy</t>
+          <t>GKS Jastrzebie</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Chojniczanka</t>
+          <t>S. Wola</t>
         </is>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>2.18</v>
+        <v>2.57</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -964,15 +964,15 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>2.46</v>
+        <v>2.64</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>22/07/2023 17:06</t>
+          <t>22/07/2023 17:59</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>3.31</v>
+        <v>3.24</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -980,15 +980,15 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>3.45</v>
+        <v>3.41</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>22/07/2023 17:35</t>
+          <t>22/07/2023 17:59</t>
         </is>
       </c>
       <c r="R6" t="n">
-        <v>3.05</v>
+        <v>2.57</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -996,16 +996,16 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>2.6</v>
+        <v>2.42</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>22/07/2023 17:06</t>
+          <t>22/07/2023 17:59</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/wisla-pulawy-chojniczanka/rc7er10t/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/gks-jastrzebie-stal-stalowa-wola/84hLxcUH/</t>
         </is>
       </c>
     </row>
@@ -1033,22 +1033,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ol. Grudziadz</t>
+          <t>Wisla Pulawy</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Sandecja Nowy S.</t>
+          <t>Chojniczanka</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>2.49</v>
+        <v>2.18</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -1056,15 +1056,15 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>2.39</v>
+        <v>2.46</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>22/07/2023 17:36</t>
+          <t>22/07/2023 17:06</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>3.26</v>
+        <v>3.31</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1072,15 +1072,15 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>3.35</v>
+        <v>3.45</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>22/07/2023 17:36</t>
+          <t>22/07/2023 17:35</t>
         </is>
       </c>
       <c r="R7" t="n">
-        <v>2.64</v>
+        <v>3.05</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1088,16 +1088,16 @@
         </is>
       </c>
       <c r="T7" t="n">
-        <v>2.82</v>
+        <v>2.6</v>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>22/07/2023 17:36</t>
+          <t>22/07/2023 17:06</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/ol-grudziadz-sandecja-nowy-s/GUiPyHqO/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/wisla-pulawy-chojniczanka/rc7er10t/</t>
         </is>
       </c>
     </row>
@@ -1125,22 +1125,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>GKS Jastrzebie</t>
+          <t>Ol. Grudziadz</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>S. Wola</t>
+          <t>Sandecja Nowy S.</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>2.57</v>
+        <v>2.49</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -1148,48 +1148,48 @@
         </is>
       </c>
       <c r="L8" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>22/07/2023 17:36</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>3.26</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>22/07/2023 14:42</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>22/07/2023 17:36</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
         <v>2.64</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>22/07/2023 17:59</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>22/07/2023 14:42</t>
         </is>
       </c>
-      <c r="P8" t="n">
-        <v>3.41</v>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>22/07/2023 17:59</t>
-        </is>
-      </c>
-      <c r="R8" t="n">
-        <v>2.57</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>22/07/2023 14:42</t>
-        </is>
-      </c>
       <c r="T8" t="n">
-        <v>2.42</v>
+        <v>2.82</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>22/07/2023 17:59</t>
+          <t>22/07/2023 17:36</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/gks-jastrzebie-stal-stalowa-wola/84hLxcUH/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/ol-grudziadz-sandecja-nowy-s/GUiPyHqO/</t>
         </is>
       </c>
     </row>
@@ -4897,22 +4897,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Zaglebie II</t>
+          <t>GKS Jastrzebie</t>
         </is>
       </c>
       <c r="G49" t="n">
+        <v>4</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Polonia Bytom</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
         <v>2</v>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Olimpia Elblag</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
       <c r="J49" t="n">
-        <v>2.01</v>
+        <v>1.85</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4920,15 +4920,15 @@
         </is>
       </c>
       <c r="L49" t="n">
-        <v>2.44</v>
+        <v>1.83</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>26/08/2023 16:30</t>
+          <t>26/08/2023 16:58</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>3.27</v>
+        <v>3.42</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4936,15 +4936,15 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>3.34</v>
+        <v>3.6</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>26/08/2023 16:30</t>
+          <t>26/08/2023 16:58</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>3.5</v>
+        <v>4.09</v>
       </c>
       <c r="S49" t="inlineStr">
         <is>
@@ -4952,16 +4952,16 @@
         </is>
       </c>
       <c r="T49" t="n">
-        <v>2.77</v>
+        <v>4.03</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>26/08/2023 16:30</t>
+          <t>26/08/2023 16:58</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/zaglebie-olimpia-elblag/QF5HX4mE/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/gks-jastrzebie-polonia-bytom/464LWO2K/</t>
         </is>
       </c>
     </row>
@@ -4989,22 +4989,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Wisla Pulawy</t>
+          <t>Pogon Siedlce</t>
         </is>
       </c>
       <c r="G50" t="n">
+        <v>3</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Sandecja Nowy S.</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
         <v>0</v>
       </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Hutnik Krakow</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>1</v>
-      </c>
       <c r="J50" t="n">
-        <v>1.78</v>
+        <v>2.28</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="L50" t="n">
-        <v>2.04</v>
+        <v>2.77</v>
       </c>
       <c r="M50" t="inlineStr">
         <is>
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>3.61</v>
+        <v>3.08</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -5028,15 +5028,15 @@
         </is>
       </c>
       <c r="P50" t="n">
-        <v>3.28</v>
+        <v>3.12</v>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>26/08/2023 16:54</t>
+          <t>26/08/2023 16:55</t>
         </is>
       </c>
       <c r="R50" t="n">
-        <v>3.99</v>
+        <v>3.09</v>
       </c>
       <c r="S50" t="inlineStr">
         <is>
@@ -5044,7 +5044,7 @@
         </is>
       </c>
       <c r="T50" t="n">
-        <v>3.62</v>
+        <v>2.56</v>
       </c>
       <c r="U50" t="inlineStr">
         <is>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/wisla-pulawy-hutnik-krakow/YLfiR2Qs/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/pogon-siedlce-sandecja-nowy-s/bT3PVrIQ/</t>
         </is>
       </c>
     </row>
@@ -5081,22 +5081,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Pogon Siedlce</t>
+          <t>Zaglebie II</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Sandecja Nowy S.</t>
+          <t>Olimpia Elblag</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>2.28</v>
+        <v>2.01</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,48 +5104,48 @@
         </is>
       </c>
       <c r="L51" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>26/08/2023 16:30</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>26/08/2023 13:13</t>
+        </is>
+      </c>
+      <c r="P51" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>26/08/2023 16:30</t>
+        </is>
+      </c>
+      <c r="R51" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>26/08/2023 13:13</t>
+        </is>
+      </c>
+      <c r="T51" t="n">
         <v>2.77</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>26/08/2023 16:56</t>
-        </is>
-      </c>
-      <c r="N51" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>26/08/2023 13:13</t>
-        </is>
-      </c>
-      <c r="P51" t="n">
-        <v>3.12</v>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>26/08/2023 16:55</t>
-        </is>
-      </c>
-      <c r="R51" t="n">
-        <v>3.09</v>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>26/08/2023 13:13</t>
-        </is>
-      </c>
-      <c r="T51" t="n">
-        <v>2.56</v>
-      </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>26/08/2023 16:56</t>
+          <t>26/08/2023 16:30</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/pogon-siedlce-sandecja-nowy-s/bT3PVrIQ/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/zaglebie-olimpia-elblag/QF5HX4mE/</t>
         </is>
       </c>
     </row>
@@ -5173,22 +5173,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>GKS Jastrzebie</t>
+          <t>Wisla Pulawy</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Polonia Bytom</t>
+          <t>Hutnik Krakow</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
-        <v>1.85</v>
+        <v>1.78</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -5196,15 +5196,15 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>1.83</v>
+        <v>2.04</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>26/08/2023 16:58</t>
+          <t>26/08/2023 16:56</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>3.42</v>
+        <v>3.61</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -5212,15 +5212,15 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>3.6</v>
+        <v>3.28</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>26/08/2023 16:58</t>
+          <t>26/08/2023 16:54</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>4.09</v>
+        <v>3.99</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
@@ -5228,16 +5228,16 @@
         </is>
       </c>
       <c r="T52" t="n">
-        <v>4.03</v>
+        <v>3.62</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>26/08/2023 16:58</t>
+          <t>26/08/2023 16:56</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/gks-jastrzebie-polonia-bytom/464LWO2K/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/wisla-pulawy-hutnik-krakow/YLfiR2Qs/</t>
         </is>
       </c>
     </row>
@@ -5541,22 +5541,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Sandecja Nowy S.</t>
+          <t>Olimpia Elblag</t>
         </is>
       </c>
       <c r="G56" t="n">
+        <v>2</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>GKS Jastrzebie</t>
+        </is>
+      </c>
+      <c r="I56" t="n">
         <v>1</v>
       </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Wisla Pulawy</t>
-        </is>
-      </c>
-      <c r="I56" t="n">
-        <v>2</v>
-      </c>
       <c r="J56" t="n">
-        <v>3.1</v>
+        <v>2.08</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
@@ -5564,15 +5564,15 @@
         </is>
       </c>
       <c r="L56" t="n">
-        <v>2.77</v>
+        <v>2.49</v>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>02/09/2023 15:46</t>
+          <t>02/09/2023 15:41</t>
         </is>
       </c>
       <c r="N56" t="n">
-        <v>3.19</v>
+        <v>3.26</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5580,15 +5580,15 @@
         </is>
       </c>
       <c r="P56" t="n">
-        <v>3.26</v>
+        <v>3.06</v>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>02/09/2023 15:46</t>
+          <t>02/09/2023 15:41</t>
         </is>
       </c>
       <c r="R56" t="n">
-        <v>2.21</v>
+        <v>3.32</v>
       </c>
       <c r="S56" t="inlineStr">
         <is>
@@ -5596,16 +5596,16 @@
         </is>
       </c>
       <c r="T56" t="n">
-        <v>2.48</v>
+        <v>2.92</v>
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>02/09/2023 15:46</t>
+          <t>02/09/2023 15:41</t>
         </is>
       </c>
       <c r="V56" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/sandecja-nowy-s-wisla-pulawy/bTuHLbfJ/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/olimpia-elblag-gks-jastrzebie/ldiSSF1n/</t>
         </is>
       </c>
     </row>
@@ -5633,22 +5633,22 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Olimpia Elblag</t>
+          <t>Sandecja Nowy S.</t>
         </is>
       </c>
       <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Wisla Pulawy</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
         <v>2</v>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>GKS Jastrzebie</t>
-        </is>
-      </c>
-      <c r="I57" t="n">
-        <v>1</v>
-      </c>
       <c r="J57" t="n">
-        <v>2.08</v>
+        <v>3.1</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
@@ -5656,48 +5656,48 @@
         </is>
       </c>
       <c r="L57" t="n">
-        <v>2.49</v>
+        <v>2.77</v>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>02/09/2023 15:41</t>
+          <t>02/09/2023 15:46</t>
         </is>
       </c>
       <c r="N57" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>02/09/2023 13:42</t>
+        </is>
+      </c>
+      <c r="P57" t="n">
         <v>3.26</v>
       </c>
-      <c r="O57" t="inlineStr">
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>02/09/2023 15:46</t>
+        </is>
+      </c>
+      <c r="R57" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="S57" t="inlineStr">
         <is>
           <t>02/09/2023 13:42</t>
         </is>
       </c>
-      <c r="P57" t="n">
-        <v>3.06</v>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>02/09/2023 15:41</t>
-        </is>
-      </c>
-      <c r="R57" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>02/09/2023 13:42</t>
-        </is>
-      </c>
       <c r="T57" t="n">
-        <v>2.92</v>
+        <v>2.48</v>
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>02/09/2023 15:41</t>
+          <t>02/09/2023 15:46</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/poland/division-2/olimpia-elblag-gks-jastrzebie/ldiSSF1n/</t>
+          <t>https://www.betexplorer.com/football/poland/division-2/sandecja-nowy-s-wisla-pulawy/bTuHLbfJ/</t>
         </is>
       </c>
     </row>
@@ -11770,6 +11770,98 @@
       <c r="V123" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/poland/division-2/pogon-siedlce-zaglebie/pr9mAP7t/</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>poland</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>division-2</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>45225.58333333334</v>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Zaglebie II</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>1</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>GKS Jastrzebie</t>
+        </is>
+      </c>
+      <c r="I124" t="n">
+        <v>1</v>
+      </c>
+      <c r="J124" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>25/10/2023 01:21</t>
+        </is>
+      </c>
+      <c r="L124" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>26/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="N124" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>25/10/2023 01:21</t>
+        </is>
+      </c>
+      <c r="P124" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>26/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="R124" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>25/10/2023 01:21</t>
+        </is>
+      </c>
+      <c r="T124" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>26/10/2023 13:59</t>
+        </is>
+      </c>
+      <c r="V124" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/poland/division-2/zaglebie-gks-jastrzebie/UVYwjMMO/</t>
         </is>
       </c>
     </row>

</xml_diff>